<commit_message>
Opciones para reducir consumo MCU
Archivo en word que explica las opciones para reducir consumo.
</commit_message>
<xml_diff>
--- a/Electronica/END_DEVICE_PCB_V1.0/Calculos Eficiencia Regulador.xlsx
+++ b/Electronica/END_DEVICE_PCB_V1.0/Calculos Eficiencia Regulador.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\PROJECTS\AEI PROJECT\AEI_IOT_V1.0\modulo\Electronica\END_DEVICE_PCB_V1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -215,56 +215,56 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,8 +548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,447 +565,447 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="14"/>
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>4.2</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <f>(B3-3.3)*1000</f>
         <v>900.00000000000034</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <f>(C3)*(0.126+0.016)</f>
         <v>127.80000000000007</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="2">
         <f>(C3)*(14.5+0.016)</f>
         <v>13064.400000000005</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <f>(C3)*(55+0.016)</f>
         <v>49514.400000000016</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3">
         <f>((55*3.3)/((55+0.016)*B3))*100</f>
         <v>78.548578075988289</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="17">
         <v>0.126</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="18">
         <v>14.5</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="18">
         <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="4">
+      <c r="A4" s="16"/>
+      <c r="B4" s="2">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="2">
         <f t="shared" ref="C4:C14" si="0">(B4-3.3)*1000</f>
         <v>799.99999999999977</v>
       </c>
-      <c r="D4" s="4">
-        <f t="shared" ref="D4:D14" si="1">(C4)*(0.126+0.016)</f>
+      <c r="D4" s="2">
+        <f t="shared" ref="D4:D8" si="1">(C4)*(0.126+0.016)</f>
         <v>113.59999999999998</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="2">
         <f t="shared" ref="E4:E8" si="2">(C4)*(14.5+0.016)</f>
         <v>11612.799999999997</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <f t="shared" ref="F4:F8" si="3">(C4)*(55+0.016)</f>
         <v>44012.799999999988</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="3">
         <f t="shared" ref="G4:G8" si="4">((55*3.3)/((55+0.016)*B4))*100</f>
         <v>80.464397053451435</v>
       </c>
-      <c r="H4" s="6"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>3.8</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="2">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <f t="shared" si="1"/>
         <v>71.000000000000014</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="2">
         <f t="shared" si="2"/>
         <v>7258</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <f t="shared" si="3"/>
         <v>27508</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <f t="shared" si="4"/>
         <v>86.816849452408121</v>
       </c>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="4">
+      <c r="A6" s="16"/>
+      <c r="B6" s="2">
         <v>3.6</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="2">
         <f t="shared" si="0"/>
         <v>300.00000000000028</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <f t="shared" si="1"/>
         <v>42.600000000000044</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="2">
         <f t="shared" si="2"/>
         <v>4354.8000000000038</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <f t="shared" si="3"/>
         <v>16504.800000000014</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <f t="shared" si="4"/>
         <v>91.640007755319658</v>
       </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="2">
         <v>3.5</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="2">
         <f t="shared" si="0"/>
         <v>200.00000000000017</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <f t="shared" si="1"/>
         <v>28.400000000000027</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="2">
         <f t="shared" si="2"/>
         <v>2903.2000000000025</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <f t="shared" si="3"/>
         <v>11003.20000000001</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="3">
         <f t="shared" si="4"/>
         <v>94.258293691185941</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="2">
         <v>3.4</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>100.00000000000009</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <f t="shared" si="1"/>
         <v>14.200000000000014</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="2">
         <f t="shared" si="2"/>
         <v>1451.6000000000013</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <f t="shared" si="3"/>
         <v>5501.6000000000049</v>
       </c>
-      <c r="G8" s="5">
-        <f t="shared" si="4"/>
+      <c r="G8" s="3">
+        <f>((55*3.3)/((55+0.016)*B8))*100</f>
         <v>97.030596446809056</v>
       </c>
-      <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="6">
         <v>4.2</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="6">
         <f t="shared" si="0"/>
         <v>900.00000000000034</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="6">
         <f>(C3)*(0.126+0.6)</f>
         <v>653.4000000000002</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="6">
         <f>(C3)*(14.5+0.6)</f>
         <v>13590.000000000005</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="6">
         <f>(C3)*(55+0.6)</f>
         <v>50040.000000000022</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="7">
         <f>((55*3.3)/((55+0.6)*B9))*100</f>
         <v>77.723535457348405</v>
       </c>
-      <c r="H9" s="14">
+      <c r="H9" s="12">
         <v>0.126</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="13">
         <v>14.5</v>
       </c>
-      <c r="J9" s="15">
+      <c r="J9" s="13">
         <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="12">
+      <c r="A10" s="11"/>
+      <c r="B10" s="6">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="6">
         <f t="shared" si="0"/>
         <v>799.99999999999977</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="6">
         <f t="shared" ref="D10:D14" si="5">(C4)*(0.126+0.6)</f>
         <v>580.79999999999984</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="6">
         <f t="shared" ref="E10:E14" si="6">(C4)*(14.5+0.6)</f>
         <v>12079.999999999996</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="6">
         <f t="shared" ref="F10:F14" si="7">(C4)*(55+0.6)</f>
         <v>44479.999999999985</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G10" s="7">
         <f t="shared" ref="G10:G14" si="8">((55*3.3)/((55+0.6)*B10))*100</f>
         <v>79.619231444113012</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="6">
         <v>3.8</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="6">
         <f t="shared" si="0"/>
         <v>500</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="6">
         <f t="shared" si="5"/>
         <v>363</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="6">
         <f t="shared" si="6"/>
         <v>7550</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="6">
         <f t="shared" si="7"/>
         <v>27800</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="7">
         <f t="shared" si="8"/>
         <v>85.90496024233245</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
-      <c r="B12" s="12">
+      <c r="A12" s="11"/>
+      <c r="B12" s="6">
         <v>3.6</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="6">
         <f t="shared" si="0"/>
         <v>300.00000000000028</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="6">
         <f t="shared" si="5"/>
         <v>217.80000000000021</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="6">
         <f t="shared" si="6"/>
         <v>4530.0000000000045</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="6">
         <f t="shared" si="7"/>
         <v>16680.000000000015</v>
       </c>
-      <c r="G12" s="13">
+      <c r="G12" s="7">
         <f t="shared" si="8"/>
         <v>90.677458033573146</v>
       </c>
-      <c r="H12" s="14"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="6">
         <v>3.5</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="6">
         <f t="shared" si="0"/>
         <v>200.00000000000017</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="6">
         <f t="shared" si="5"/>
         <v>145.20000000000013</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="6">
         <f t="shared" si="6"/>
         <v>3020.0000000000027</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="6">
         <f t="shared" si="7"/>
         <v>11120.000000000009</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="7">
         <f t="shared" si="8"/>
         <v>93.268242548818094</v>
       </c>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="6">
         <v>3.4</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="6">
         <f t="shared" si="0"/>
         <v>100.00000000000009</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="6">
         <f t="shared" si="5"/>
         <v>72.600000000000065</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="6">
         <f t="shared" si="6"/>
         <v>1510.0000000000014</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="6">
         <f t="shared" si="7"/>
         <v>5560.0000000000045</v>
       </c>
-      <c r="G14" s="13">
-        <f t="shared" si="8"/>
+      <c r="G14" s="7">
+        <f>((55*3.3)/((55+0.6)*B14))*100</f>
         <v>96.011426153195089</v>
       </c>
-      <c r="H14" s="14"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="H9:H14"/>
-    <mergeCell ref="I9:I14"/>
-    <mergeCell ref="J9:J14"/>
-    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="H3:H8"/>
+    <mergeCell ref="I3:I8"/>
+    <mergeCell ref="J3:J8"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="D1:F1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="H3:H8"/>
-    <mergeCell ref="I3:I8"/>
-    <mergeCell ref="J3:J8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="H9:H14"/>
+    <mergeCell ref="I9:I14"/>
+    <mergeCell ref="J9:J14"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>